<commit_message>
4-27_1744 word addin datastructure
</commit_message>
<xml_diff>
--- a/program_files/note_template_cache.xlsx
+++ b/program_files/note_template_cache.xlsx
@@ -532,22 +532,50 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
           <t>货币资金</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>货币资金</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>合计</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>年初余额</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>合计</t>
+        </is>
+      </c>
+      <c r="I2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>年末余额</t>
+        </is>
+      </c>
+      <c r="K2" t="n">
+        <v>0</v>
+      </c>
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr"/>
       <c r="N2" t="inlineStr"/>
@@ -559,22 +587,50 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
           <t>货币资金-现金</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>货币资金</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>现金</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>年初余额</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>现金</t>
+        </is>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>年末余额</t>
+        </is>
+      </c>
+      <c r="K3" t="n">
+        <v>0</v>
+      </c>
       <c r="L3" t="inlineStr"/>
       <c r="M3" t="inlineStr"/>
       <c r="N3" t="inlineStr"/>
@@ -586,22 +642,50 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
           <t>货币资金-银行存款</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>货币资金</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>银行存款</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>年初余额</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>银行存款</t>
+        </is>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>年末余额</t>
+        </is>
+      </c>
+      <c r="K4" t="n">
+        <v>0</v>
+      </c>
       <c r="L4" t="inlineStr"/>
       <c r="M4" t="inlineStr"/>
       <c r="N4" t="inlineStr"/>
@@ -613,7 +697,7 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -640,7 +724,7 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -667,7 +751,7 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -694,22 +778,50 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
           <t>应收票据</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>应收票据</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>合计</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>年初余额</t>
+        </is>
+      </c>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>合计</t>
+        </is>
+      </c>
+      <c r="I8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>年末余额</t>
+        </is>
+      </c>
+      <c r="K8" t="n">
+        <v>0</v>
+      </c>
       <c r="L8" t="inlineStr"/>
       <c r="M8" t="inlineStr"/>
       <c r="N8" t="inlineStr"/>
@@ -721,22 +833,50 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
           <t>应收账款</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr"/>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>应收账款</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>合计</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>年初余额</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>合计</t>
+        </is>
+      </c>
+      <c r="I9" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>年末余额</t>
+        </is>
+      </c>
+      <c r="K9" t="n">
+        <v>0</v>
+      </c>
       <c r="L9" t="inlineStr"/>
       <c r="M9" t="inlineStr"/>
       <c r="N9" t="inlineStr"/>
@@ -748,22 +888,50 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
           <t>预付款项</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>预付款项</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>合计</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>年初余额</t>
+        </is>
+      </c>
+      <c r="G10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>合计</t>
+        </is>
+      </c>
+      <c r="I10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>年末余额</t>
+        </is>
+      </c>
+      <c r="K10" t="n">
+        <v>0</v>
+      </c>
       <c r="L10" t="inlineStr"/>
       <c r="M10" t="inlineStr"/>
       <c r="N10" t="inlineStr"/>
@@ -775,7 +943,7 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -802,7 +970,7 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -829,22 +997,50 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
           <t>其他应收款</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr"/>
-      <c r="J13" t="inlineStr"/>
-      <c r="K13" t="inlineStr"/>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>其他应收款</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>合计</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>年初余额</t>
+        </is>
+      </c>
+      <c r="G13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>合计</t>
+        </is>
+      </c>
+      <c r="I13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>年末余额</t>
+        </is>
+      </c>
+      <c r="K13" t="n">
+        <v>0</v>
+      </c>
       <c r="L13" t="inlineStr"/>
       <c r="M13" t="inlineStr"/>
       <c r="N13" t="inlineStr"/>
@@ -856,22 +1052,50 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
           <t>存货</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr"/>
-      <c r="D14" t="inlineStr"/>
-      <c r="E14" t="inlineStr"/>
-      <c r="F14" t="inlineStr"/>
-      <c r="G14" t="inlineStr"/>
-      <c r="H14" t="inlineStr"/>
-      <c r="I14" t="inlineStr"/>
-      <c r="J14" t="inlineStr"/>
-      <c r="K14" t="inlineStr"/>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>存货</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>合计</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>年初余额</t>
+        </is>
+      </c>
+      <c r="G14" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>合计</t>
+        </is>
+      </c>
+      <c r="I14" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>年末余额</t>
+        </is>
+      </c>
+      <c r="K14" t="n">
+        <v>0</v>
+      </c>
       <c r="L14" t="inlineStr"/>
       <c r="M14" t="inlineStr"/>
       <c r="N14" t="inlineStr"/>
@@ -883,7 +1107,7 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -910,7 +1134,7 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -937,22 +1161,50 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
           <t>其他流动资产</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr"/>
-      <c r="D17" t="inlineStr"/>
-      <c r="E17" t="inlineStr"/>
-      <c r="F17" t="inlineStr"/>
-      <c r="G17" t="inlineStr"/>
-      <c r="H17" t="inlineStr"/>
-      <c r="I17" t="inlineStr"/>
-      <c r="J17" t="inlineStr"/>
-      <c r="K17" t="inlineStr"/>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>其他流动资产</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>合计</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>年初余额</t>
+        </is>
+      </c>
+      <c r="G17" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>合计</t>
+        </is>
+      </c>
+      <c r="I17" t="n">
+        <v>0</v>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>年末余额</t>
+        </is>
+      </c>
+      <c r="K17" t="n">
+        <v>0</v>
+      </c>
       <c r="L17" t="inlineStr"/>
       <c r="M17" t="inlineStr"/>
       <c r="N17" t="inlineStr"/>
@@ -964,7 +1216,7 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -991,7 +1243,7 @@
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -1018,7 +1270,7 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -1045,7 +1297,7 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -1072,7 +1324,7 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
@@ -1099,22 +1351,50 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
           <t>固定资产</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr"/>
-      <c r="D23" t="inlineStr"/>
-      <c r="E23" t="inlineStr"/>
-      <c r="F23" t="inlineStr"/>
-      <c r="G23" t="inlineStr"/>
-      <c r="H23" t="inlineStr"/>
-      <c r="I23" t="inlineStr"/>
-      <c r="J23" t="inlineStr"/>
-      <c r="K23" t="inlineStr"/>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>固定资产净值</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>合计</t>
+        </is>
+      </c>
+      <c r="E23" t="n">
+        <v>0</v>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>年初余额</t>
+        </is>
+      </c>
+      <c r="G23" t="n">
+        <v>0</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>合计</t>
+        </is>
+      </c>
+      <c r="I23" t="n">
+        <v>0</v>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>年末余额</t>
+        </is>
+      </c>
+      <c r="K23" t="n">
+        <v>0</v>
+      </c>
       <c r="L23" t="inlineStr"/>
       <c r="M23" t="inlineStr"/>
       <c r="N23" t="inlineStr"/>
@@ -1126,22 +1406,50 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
           <t>在建工程</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr"/>
-      <c r="D24" t="inlineStr"/>
-      <c r="E24" t="inlineStr"/>
-      <c r="F24" t="inlineStr"/>
-      <c r="G24" t="inlineStr"/>
-      <c r="H24" t="inlineStr"/>
-      <c r="I24" t="inlineStr"/>
-      <c r="J24" t="inlineStr"/>
-      <c r="K24" t="inlineStr"/>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>在建工程</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>合计</t>
+        </is>
+      </c>
+      <c r="E24" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>年初余额</t>
+        </is>
+      </c>
+      <c r="G24" t="n">
+        <v>0</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>合计</t>
+        </is>
+      </c>
+      <c r="I24" t="n">
+        <v>0</v>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>年末余额</t>
+        </is>
+      </c>
+      <c r="K24" t="n">
+        <v>0</v>
+      </c>
       <c r="L24" t="inlineStr"/>
       <c r="M24" t="inlineStr"/>
       <c r="N24" t="inlineStr"/>
@@ -1153,7 +1461,7 @@
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
@@ -1180,7 +1488,7 @@
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
@@ -1207,7 +1515,7 @@
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
@@ -1234,7 +1542,7 @@
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
@@ -1261,22 +1569,50 @@
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
           <t>无形资产</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr"/>
-      <c r="D29" t="inlineStr"/>
-      <c r="E29" t="inlineStr"/>
-      <c r="F29" t="inlineStr"/>
-      <c r="G29" t="inlineStr"/>
-      <c r="H29" t="inlineStr"/>
-      <c r="I29" t="inlineStr"/>
-      <c r="J29" t="inlineStr"/>
-      <c r="K29" t="inlineStr"/>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>无形资产</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>合计</t>
+        </is>
+      </c>
+      <c r="E29" t="n">
+        <v>0</v>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>年初余额</t>
+        </is>
+      </c>
+      <c r="G29" t="n">
+        <v>0</v>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>合计</t>
+        </is>
+      </c>
+      <c r="I29" t="n">
+        <v>0</v>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>年末余额</t>
+        </is>
+      </c>
+      <c r="K29" t="n">
+        <v>0</v>
+      </c>
       <c r="L29" t="inlineStr"/>
       <c r="M29" t="inlineStr"/>
       <c r="N29" t="inlineStr"/>
@@ -1288,7 +1624,7 @@
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
@@ -1315,7 +1651,7 @@
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
@@ -1342,22 +1678,50 @@
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
           <t>长期待摊费用</t>
         </is>
       </c>
-      <c r="C32" t="inlineStr"/>
-      <c r="D32" t="inlineStr"/>
-      <c r="E32" t="inlineStr"/>
-      <c r="F32" t="inlineStr"/>
-      <c r="G32" t="inlineStr"/>
-      <c r="H32" t="inlineStr"/>
-      <c r="I32" t="inlineStr"/>
-      <c r="J32" t="inlineStr"/>
-      <c r="K32" t="inlineStr"/>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>长期待摊费用</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>合计</t>
+        </is>
+      </c>
+      <c r="E32" t="n">
+        <v>0</v>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>年初余额</t>
+        </is>
+      </c>
+      <c r="G32" t="n">
+        <v>0</v>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>合计</t>
+        </is>
+      </c>
+      <c r="I32" t="n">
+        <v>0</v>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>年末余额</t>
+        </is>
+      </c>
+      <c r="K32" t="n">
+        <v>0</v>
+      </c>
       <c r="L32" t="inlineStr"/>
       <c r="M32" t="inlineStr"/>
       <c r="N32" t="inlineStr"/>
@@ -1369,7 +1733,7 @@
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
@@ -1396,7 +1760,7 @@
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
@@ -1423,22 +1787,50 @@
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
           <t>短期借款</t>
         </is>
       </c>
-      <c r="C35" t="inlineStr"/>
-      <c r="D35" t="inlineStr"/>
-      <c r="E35" t="inlineStr"/>
-      <c r="F35" t="inlineStr"/>
-      <c r="G35" t="inlineStr"/>
-      <c r="H35" t="inlineStr"/>
-      <c r="I35" t="inlineStr"/>
-      <c r="J35" t="inlineStr"/>
-      <c r="K35" t="inlineStr"/>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>短期借款</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>合计</t>
+        </is>
+      </c>
+      <c r="E35" t="n">
+        <v>0</v>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>年初余额</t>
+        </is>
+      </c>
+      <c r="G35" t="n">
+        <v>0</v>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>合计</t>
+        </is>
+      </c>
+      <c r="I35" t="n">
+        <v>0</v>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>年末余额</t>
+        </is>
+      </c>
+      <c r="K35" t="n">
+        <v>0</v>
+      </c>
       <c r="L35" t="inlineStr"/>
       <c r="M35" t="inlineStr"/>
       <c r="N35" t="inlineStr"/>
@@ -1450,7 +1842,7 @@
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
@@ -1477,7 +1869,7 @@
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
@@ -1504,7 +1896,7 @@
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
@@ -1531,22 +1923,50 @@
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
           <t>应付账款</t>
         </is>
       </c>
-      <c r="C39" t="inlineStr"/>
-      <c r="D39" t="inlineStr"/>
-      <c r="E39" t="inlineStr"/>
-      <c r="F39" t="inlineStr"/>
-      <c r="G39" t="inlineStr"/>
-      <c r="H39" t="inlineStr"/>
-      <c r="I39" t="inlineStr"/>
-      <c r="J39" t="inlineStr"/>
-      <c r="K39" t="inlineStr"/>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>应付账款</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>应付账款</t>
+        </is>
+      </c>
+      <c r="E39" t="n">
+        <v>0</v>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>年初余额</t>
+        </is>
+      </c>
+      <c r="G39" t="n">
+        <v>0</v>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>合计</t>
+        </is>
+      </c>
+      <c r="I39" t="n">
+        <v>0</v>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>年末余额</t>
+        </is>
+      </c>
+      <c r="K39" t="n">
+        <v>0</v>
+      </c>
       <c r="L39" t="inlineStr"/>
       <c r="M39" t="inlineStr"/>
       <c r="N39" t="inlineStr"/>
@@ -1558,22 +1978,50 @@
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
           <t>预收款项</t>
         </is>
       </c>
-      <c r="C40" t="inlineStr"/>
-      <c r="D40" t="inlineStr"/>
-      <c r="E40" t="inlineStr"/>
-      <c r="F40" t="inlineStr"/>
-      <c r="G40" t="inlineStr"/>
-      <c r="H40" t="inlineStr"/>
-      <c r="I40" t="inlineStr"/>
-      <c r="J40" t="inlineStr"/>
-      <c r="K40" t="inlineStr"/>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>预收款项</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>预收账款</t>
+        </is>
+      </c>
+      <c r="E40" t="n">
+        <v>0</v>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>年初余额</t>
+        </is>
+      </c>
+      <c r="G40" t="n">
+        <v>0</v>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>合计</t>
+        </is>
+      </c>
+      <c r="I40" t="n">
+        <v>0</v>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>年末余额</t>
+        </is>
+      </c>
+      <c r="K40" t="n">
+        <v>0</v>
+      </c>
       <c r="L40" t="inlineStr"/>
       <c r="M40" t="inlineStr"/>
       <c r="N40" t="inlineStr"/>
@@ -1585,22 +2033,50 @@
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
           <t>应付职工薪酬</t>
         </is>
       </c>
-      <c r="C41" t="inlineStr"/>
-      <c r="D41" t="inlineStr"/>
-      <c r="E41" t="inlineStr"/>
-      <c r="F41" t="inlineStr"/>
-      <c r="G41" t="inlineStr"/>
-      <c r="H41" t="inlineStr"/>
-      <c r="I41" t="inlineStr"/>
-      <c r="J41" t="inlineStr"/>
-      <c r="K41" t="inlineStr"/>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>应付职工薪酬</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>合计</t>
+        </is>
+      </c>
+      <c r="E41" t="n">
+        <v>0</v>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>年初余额</t>
+        </is>
+      </c>
+      <c r="G41" t="n">
+        <v>0</v>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>合计</t>
+        </is>
+      </c>
+      <c r="I41" t="n">
+        <v>0</v>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>年末余额</t>
+        </is>
+      </c>
+      <c r="K41" t="n">
+        <v>0</v>
+      </c>
       <c r="L41" t="inlineStr"/>
       <c r="M41" t="inlineStr"/>
       <c r="N41" t="inlineStr"/>
@@ -1612,22 +2088,50 @@
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
           <t>应交税费</t>
         </is>
       </c>
-      <c r="C42" t="inlineStr"/>
-      <c r="D42" t="inlineStr"/>
-      <c r="E42" t="inlineStr"/>
-      <c r="F42" t="inlineStr"/>
-      <c r="G42" t="inlineStr"/>
-      <c r="H42" t="inlineStr"/>
-      <c r="I42" t="inlineStr"/>
-      <c r="J42" t="inlineStr"/>
-      <c r="K42" t="inlineStr"/>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>应交税费</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>合计</t>
+        </is>
+      </c>
+      <c r="E42" t="n">
+        <v>0</v>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>年初余额</t>
+        </is>
+      </c>
+      <c r="G42" t="n">
+        <v>0</v>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>合计</t>
+        </is>
+      </c>
+      <c r="I42" t="n">
+        <v>0</v>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>年末余额</t>
+        </is>
+      </c>
+      <c r="K42" t="n">
+        <v>0</v>
+      </c>
       <c r="L42" t="inlineStr"/>
       <c r="M42" t="inlineStr"/>
       <c r="N42" t="inlineStr"/>
@@ -1639,7 +2143,7 @@
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
@@ -1666,7 +2170,7 @@
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
@@ -1693,22 +2197,50 @@
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
           <t>其他应付款</t>
         </is>
       </c>
-      <c r="C45" t="inlineStr"/>
-      <c r="D45" t="inlineStr"/>
-      <c r="E45" t="inlineStr"/>
-      <c r="F45" t="inlineStr"/>
-      <c r="G45" t="inlineStr"/>
-      <c r="H45" t="inlineStr"/>
-      <c r="I45" t="inlineStr"/>
-      <c r="J45" t="inlineStr"/>
-      <c r="K45" t="inlineStr"/>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>其他应付款</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>合计</t>
+        </is>
+      </c>
+      <c r="E45" t="n">
+        <v>0</v>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>年初余额</t>
+        </is>
+      </c>
+      <c r="G45" t="n">
+        <v>0</v>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>合计</t>
+        </is>
+      </c>
+      <c r="I45" t="n">
+        <v>0</v>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>年末余额</t>
+        </is>
+      </c>
+      <c r="K45" t="n">
+        <v>0</v>
+      </c>
       <c r="L45" t="inlineStr"/>
       <c r="M45" t="inlineStr"/>
       <c r="N45" t="inlineStr"/>
@@ -1720,7 +2252,7 @@
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
@@ -1747,7 +2279,7 @@
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
@@ -1774,7 +2306,7 @@
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
@@ -1801,7 +2333,7 @@
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
@@ -1828,7 +2360,7 @@
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
@@ -1855,7 +2387,7 @@
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
@@ -1882,7 +2414,7 @@
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
@@ -1909,7 +2441,7 @@
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
@@ -1936,7 +2468,7 @@
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
@@ -1963,7 +2495,7 @@
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
@@ -1990,7 +2522,7 @@
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
@@ -2017,7 +2549,7 @@
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
@@ -2044,7 +2576,7 @@
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
@@ -2071,7 +2603,7 @@
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
@@ -2098,7 +2630,7 @@
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
@@ -2125,22 +2657,50 @@
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
           <t>实收资本</t>
         </is>
       </c>
-      <c r="C61" t="inlineStr"/>
-      <c r="D61" t="inlineStr"/>
-      <c r="E61" t="inlineStr"/>
-      <c r="F61" t="inlineStr"/>
-      <c r="G61" t="inlineStr"/>
-      <c r="H61" t="inlineStr"/>
-      <c r="I61" t="inlineStr"/>
-      <c r="J61" t="inlineStr"/>
-      <c r="K61" t="inlineStr"/>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>实收资本</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>合计</t>
+        </is>
+      </c>
+      <c r="E61" t="n">
+        <v>0</v>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>年初余额</t>
+        </is>
+      </c>
+      <c r="G61" t="n">
+        <v>0</v>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>合计</t>
+        </is>
+      </c>
+      <c r="I61" t="n">
+        <v>0</v>
+      </c>
+      <c r="J61" t="inlineStr">
+        <is>
+          <t>年末余额</t>
+        </is>
+      </c>
+      <c r="K61" t="n">
+        <v>0</v>
+      </c>
       <c r="L61" t="inlineStr"/>
       <c r="M61" t="inlineStr"/>
       <c r="N61" t="inlineStr"/>
@@ -2152,7 +2712,7 @@
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
@@ -2179,7 +2739,7 @@
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
@@ -2206,7 +2766,7 @@
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
@@ -2233,7 +2793,7 @@
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
@@ -2260,7 +2820,7 @@
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
@@ -2287,7 +2847,7 @@
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
@@ -2314,7 +2874,7 @@
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
@@ -2341,22 +2901,50 @@
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B69" t="inlineStr">
         <is>
           <t>盈余公积</t>
         </is>
       </c>
-      <c r="C69" t="inlineStr"/>
-      <c r="D69" t="inlineStr"/>
-      <c r="E69" t="inlineStr"/>
-      <c r="F69" t="inlineStr"/>
-      <c r="G69" t="inlineStr"/>
-      <c r="H69" t="inlineStr"/>
-      <c r="I69" t="inlineStr"/>
-      <c r="J69" t="inlineStr"/>
-      <c r="K69" t="inlineStr"/>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>盈余公积</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>合计</t>
+        </is>
+      </c>
+      <c r="E69" t="n">
+        <v>0</v>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>年初余额</t>
+        </is>
+      </c>
+      <c r="G69" t="n">
+        <v>0</v>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>合计</t>
+        </is>
+      </c>
+      <c r="I69" t="n">
+        <v>0</v>
+      </c>
+      <c r="J69" t="inlineStr">
+        <is>
+          <t>年末余额</t>
+        </is>
+      </c>
+      <c r="K69" t="n">
+        <v>0</v>
+      </c>
       <c r="L69" t="inlineStr"/>
       <c r="M69" t="inlineStr"/>
       <c r="N69" t="inlineStr"/>
@@ -2368,22 +2956,50 @@
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
           <t>未分配利润</t>
         </is>
       </c>
-      <c r="C70" t="inlineStr"/>
-      <c r="D70" t="inlineStr"/>
-      <c r="E70" t="inlineStr"/>
-      <c r="F70" t="inlineStr"/>
-      <c r="G70" t="inlineStr"/>
-      <c r="H70" t="inlineStr"/>
-      <c r="I70" t="inlineStr"/>
-      <c r="J70" t="inlineStr"/>
-      <c r="K70" t="inlineStr"/>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>未分配利润</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>本年年末余额</t>
+        </is>
+      </c>
+      <c r="E70" t="n">
+        <v>0</v>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>2021年</t>
+        </is>
+      </c>
+      <c r="G70" t="n">
+        <v>0</v>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>本年年末余额</t>
+        </is>
+      </c>
+      <c r="I70" t="n">
+        <v>0</v>
+      </c>
+      <c r="J70" t="inlineStr">
+        <is>
+          <t>2022年</t>
+        </is>
+      </c>
+      <c r="K70" t="n">
+        <v>0</v>
+      </c>
       <c r="L70" t="inlineStr"/>
       <c r="M70" t="inlineStr"/>
       <c r="N70" t="inlineStr"/>
@@ -2395,7 +3011,7 @@
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
@@ -2422,7 +3038,7 @@
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
@@ -2449,7 +3065,7 @@
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
@@ -2476,7 +3092,7 @@
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
@@ -2503,7 +3119,7 @@
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
@@ -2530,7 +3146,7 @@
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B76" t="inlineStr">
         <is>
@@ -2557,7 +3173,7 @@
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B77" t="inlineStr">
         <is>
@@ -2584,7 +3200,7 @@
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B78" t="inlineStr">
         <is>
@@ -2611,7 +3227,7 @@
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
@@ -2638,7 +3254,7 @@
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
@@ -2665,7 +3281,7 @@
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
@@ -2692,7 +3308,7 @@
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
@@ -2719,7 +3335,7 @@
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
@@ -2746,7 +3362,7 @@
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
@@ -2762,18 +3378,44 @@
       <c r="I84" t="inlineStr"/>
       <c r="J84" t="inlineStr"/>
       <c r="K84" t="inlineStr"/>
-      <c r="L84" t="inlineStr"/>
-      <c r="M84" t="inlineStr"/>
-      <c r="N84" t="inlineStr"/>
-      <c r="O84" t="inlineStr"/>
-      <c r="P84" t="inlineStr"/>
-      <c r="Q84" t="inlineStr"/>
-      <c r="R84" t="inlineStr"/>
-      <c r="S84" t="inlineStr"/>
+      <c r="L84" t="inlineStr">
+        <is>
+          <t>营业收支</t>
+        </is>
+      </c>
+      <c r="M84" t="inlineStr">
+        <is>
+          <t>主营业务</t>
+        </is>
+      </c>
+      <c r="N84" t="n">
+        <v>0</v>
+      </c>
+      <c r="O84" t="inlineStr">
+        <is>
+          <t>2021年</t>
+        </is>
+      </c>
+      <c r="P84" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q84" t="inlineStr">
+        <is>
+          <t>主营业务</t>
+        </is>
+      </c>
+      <c r="R84" t="n">
+        <v>0</v>
+      </c>
+      <c r="S84" t="inlineStr">
+        <is>
+          <t>2022年</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
@@ -2789,18 +3431,44 @@
       <c r="I85" t="inlineStr"/>
       <c r="J85" t="inlineStr"/>
       <c r="K85" t="inlineStr"/>
-      <c r="L85" t="inlineStr"/>
-      <c r="M85" t="inlineStr"/>
-      <c r="N85" t="inlineStr"/>
-      <c r="O85" t="inlineStr"/>
-      <c r="P85" t="inlineStr"/>
-      <c r="Q85" t="inlineStr"/>
-      <c r="R85" t="inlineStr"/>
-      <c r="S85" t="inlineStr"/>
+      <c r="L85" t="inlineStr">
+        <is>
+          <t>营业收支</t>
+        </is>
+      </c>
+      <c r="M85" t="inlineStr">
+        <is>
+          <t>其他业务</t>
+        </is>
+      </c>
+      <c r="N85" t="n">
+        <v>0</v>
+      </c>
+      <c r="O85" t="inlineStr">
+        <is>
+          <t>2021年</t>
+        </is>
+      </c>
+      <c r="P85" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q85" t="inlineStr">
+        <is>
+          <t>其他业务</t>
+        </is>
+      </c>
+      <c r="R85" t="n">
+        <v>0</v>
+      </c>
+      <c r="S85" t="inlineStr">
+        <is>
+          <t>2022年</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B86" t="inlineStr">
         <is>
@@ -2827,7 +3495,7 @@
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B87" t="inlineStr">
         <is>
@@ -2843,18 +3511,44 @@
       <c r="I87" t="inlineStr"/>
       <c r="J87" t="inlineStr"/>
       <c r="K87" t="inlineStr"/>
-      <c r="L87" t="inlineStr"/>
-      <c r="M87" t="inlineStr"/>
-      <c r="N87" t="inlineStr"/>
-      <c r="O87" t="inlineStr"/>
-      <c r="P87" t="inlineStr"/>
-      <c r="Q87" t="inlineStr"/>
-      <c r="R87" t="inlineStr"/>
-      <c r="S87" t="inlineStr"/>
+      <c r="L87" t="inlineStr">
+        <is>
+          <t>营业收支</t>
+        </is>
+      </c>
+      <c r="M87" t="inlineStr">
+        <is>
+          <t>主营业务</t>
+        </is>
+      </c>
+      <c r="N87" t="n">
+        <v>0</v>
+      </c>
+      <c r="O87" t="inlineStr">
+        <is>
+          <t>2021年</t>
+        </is>
+      </c>
+      <c r="P87" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q87" t="inlineStr">
+        <is>
+          <t>主营业务</t>
+        </is>
+      </c>
+      <c r="R87" t="n">
+        <v>0</v>
+      </c>
+      <c r="S87" t="inlineStr">
+        <is>
+          <t>2022年</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B88" t="inlineStr">
         <is>
@@ -2870,18 +3564,44 @@
       <c r="I88" t="inlineStr"/>
       <c r="J88" t="inlineStr"/>
       <c r="K88" t="inlineStr"/>
-      <c r="L88" t="inlineStr"/>
-      <c r="M88" t="inlineStr"/>
-      <c r="N88" t="inlineStr"/>
-      <c r="O88" t="inlineStr"/>
-      <c r="P88" t="inlineStr"/>
-      <c r="Q88" t="inlineStr"/>
-      <c r="R88" t="inlineStr"/>
-      <c r="S88" t="inlineStr"/>
+      <c r="L88" t="inlineStr">
+        <is>
+          <t>营业收支</t>
+        </is>
+      </c>
+      <c r="M88" t="inlineStr">
+        <is>
+          <t>其他业务</t>
+        </is>
+      </c>
+      <c r="N88" t="n">
+        <v>0</v>
+      </c>
+      <c r="O88" t="inlineStr">
+        <is>
+          <t>2021年</t>
+        </is>
+      </c>
+      <c r="P88" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q88" t="inlineStr">
+        <is>
+          <t>其他业务</t>
+        </is>
+      </c>
+      <c r="R88" t="n">
+        <v>0</v>
+      </c>
+      <c r="S88" t="inlineStr">
+        <is>
+          <t>2022年</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B89" t="inlineStr">
         <is>
@@ -2897,18 +3617,44 @@
       <c r="I89" t="inlineStr"/>
       <c r="J89" t="inlineStr"/>
       <c r="K89" t="inlineStr"/>
-      <c r="L89" t="inlineStr"/>
-      <c r="M89" t="inlineStr"/>
-      <c r="N89" t="inlineStr"/>
-      <c r="O89" t="inlineStr"/>
-      <c r="P89" t="inlineStr"/>
-      <c r="Q89" t="inlineStr"/>
-      <c r="R89" t="inlineStr"/>
-      <c r="S89" t="inlineStr"/>
+      <c r="L89" t="inlineStr">
+        <is>
+          <t>税金及附加</t>
+        </is>
+      </c>
+      <c r="M89" t="inlineStr">
+        <is>
+          <t>合计</t>
+        </is>
+      </c>
+      <c r="N89" t="n">
+        <v>0</v>
+      </c>
+      <c r="O89" t="inlineStr">
+        <is>
+          <t>2021年</t>
+        </is>
+      </c>
+      <c r="P89" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q89" t="inlineStr">
+        <is>
+          <t>合计</t>
+        </is>
+      </c>
+      <c r="R89" t="n">
+        <v>0</v>
+      </c>
+      <c r="S89" t="inlineStr">
+        <is>
+          <t>2022年</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B90" t="inlineStr">
         <is>
@@ -2924,18 +3670,44 @@
       <c r="I90" t="inlineStr"/>
       <c r="J90" t="inlineStr"/>
       <c r="K90" t="inlineStr"/>
-      <c r="L90" t="inlineStr"/>
-      <c r="M90" t="inlineStr"/>
-      <c r="N90" t="inlineStr"/>
-      <c r="O90" t="inlineStr"/>
-      <c r="P90" t="inlineStr"/>
-      <c r="Q90" t="inlineStr"/>
-      <c r="R90" t="inlineStr"/>
-      <c r="S90" t="inlineStr"/>
+      <c r="L90" t="inlineStr">
+        <is>
+          <t>销售费用</t>
+        </is>
+      </c>
+      <c r="M90" t="inlineStr">
+        <is>
+          <t>全年发生额</t>
+        </is>
+      </c>
+      <c r="N90" t="n">
+        <v>0</v>
+      </c>
+      <c r="O90" t="inlineStr">
+        <is>
+          <t>2021年</t>
+        </is>
+      </c>
+      <c r="P90" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q90" t="inlineStr">
+        <is>
+          <t>全年发生额</t>
+        </is>
+      </c>
+      <c r="R90" t="n">
+        <v>0</v>
+      </c>
+      <c r="S90" t="inlineStr">
+        <is>
+          <t>2022年</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B91" t="inlineStr">
         <is>
@@ -2951,18 +3723,44 @@
       <c r="I91" t="inlineStr"/>
       <c r="J91" t="inlineStr"/>
       <c r="K91" t="inlineStr"/>
-      <c r="L91" t="inlineStr"/>
-      <c r="M91" t="inlineStr"/>
-      <c r="N91" t="inlineStr"/>
-      <c r="O91" t="inlineStr"/>
-      <c r="P91" t="inlineStr"/>
-      <c r="Q91" t="inlineStr"/>
-      <c r="R91" t="inlineStr"/>
-      <c r="S91" t="inlineStr"/>
+      <c r="L91" t="inlineStr">
+        <is>
+          <t>管理费用</t>
+        </is>
+      </c>
+      <c r="M91" t="inlineStr">
+        <is>
+          <t>全年发生额</t>
+        </is>
+      </c>
+      <c r="N91" t="n">
+        <v>0</v>
+      </c>
+      <c r="O91" t="inlineStr">
+        <is>
+          <t>2021年</t>
+        </is>
+      </c>
+      <c r="P91" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q91" t="inlineStr">
+        <is>
+          <t>全年发生额</t>
+        </is>
+      </c>
+      <c r="R91" t="n">
+        <v>0</v>
+      </c>
+      <c r="S91" t="inlineStr">
+        <is>
+          <t>2022年</t>
+        </is>
+      </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B92" t="inlineStr">
         <is>
@@ -2978,18 +3776,44 @@
       <c r="I92" t="inlineStr"/>
       <c r="J92" t="inlineStr"/>
       <c r="K92" t="inlineStr"/>
-      <c r="L92" t="inlineStr"/>
-      <c r="M92" t="inlineStr"/>
-      <c r="N92" t="inlineStr"/>
-      <c r="O92" t="inlineStr"/>
-      <c r="P92" t="inlineStr"/>
-      <c r="Q92" t="inlineStr"/>
-      <c r="R92" t="inlineStr"/>
-      <c r="S92" t="inlineStr"/>
+      <c r="L92" t="inlineStr">
+        <is>
+          <t>财务费用</t>
+        </is>
+      </c>
+      <c r="M92" t="inlineStr">
+        <is>
+          <t>合计</t>
+        </is>
+      </c>
+      <c r="N92" t="n">
+        <v>0</v>
+      </c>
+      <c r="O92" t="inlineStr">
+        <is>
+          <t>2021年</t>
+        </is>
+      </c>
+      <c r="P92" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q92" t="inlineStr">
+        <is>
+          <t>合计</t>
+        </is>
+      </c>
+      <c r="R92" t="n">
+        <v>0</v>
+      </c>
+      <c r="S92" t="inlineStr">
+        <is>
+          <t>2022年</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B93" t="inlineStr">
         <is>
@@ -3016,7 +3840,7 @@
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B94" t="inlineStr">
         <is>
@@ -3043,7 +3867,7 @@
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B95" t="inlineStr">
         <is>
@@ -3070,7 +3894,7 @@
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B96" t="inlineStr">
         <is>
@@ -3097,7 +3921,7 @@
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B97" t="inlineStr">
         <is>
@@ -3124,7 +3948,7 @@
     </row>
     <row r="98">
       <c r="A98" s="1" t="n">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B98" t="inlineStr">
         <is>
@@ -3140,18 +3964,44 @@
       <c r="I98" t="inlineStr"/>
       <c r="J98" t="inlineStr"/>
       <c r="K98" t="inlineStr"/>
-      <c r="L98" t="inlineStr"/>
-      <c r="M98" t="inlineStr"/>
-      <c r="N98" t="inlineStr"/>
-      <c r="O98" t="inlineStr"/>
-      <c r="P98" t="inlineStr"/>
-      <c r="Q98" t="inlineStr"/>
-      <c r="R98" t="inlineStr"/>
-      <c r="S98" t="inlineStr"/>
+      <c r="L98" t="inlineStr">
+        <is>
+          <t>其他收益</t>
+        </is>
+      </c>
+      <c r="M98" t="inlineStr">
+        <is>
+          <t>合计</t>
+        </is>
+      </c>
+      <c r="N98" t="n">
+        <v>0</v>
+      </c>
+      <c r="O98" t="inlineStr">
+        <is>
+          <t>2021年</t>
+        </is>
+      </c>
+      <c r="P98" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q98" t="inlineStr">
+        <is>
+          <t>合计</t>
+        </is>
+      </c>
+      <c r="R98" t="n">
+        <v>0</v>
+      </c>
+      <c r="S98" t="inlineStr">
+        <is>
+          <t>2022年</t>
+        </is>
+      </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="n">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B99" t="inlineStr">
         <is>
@@ -3178,7 +4028,7 @@
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B100" t="inlineStr">
         <is>
@@ -3205,7 +4055,7 @@
     </row>
     <row r="101">
       <c r="A101" s="1" t="n">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B101" t="inlineStr">
         <is>
@@ -3221,18 +4071,44 @@
       <c r="I101" t="inlineStr"/>
       <c r="J101" t="inlineStr"/>
       <c r="K101" t="inlineStr"/>
-      <c r="L101" t="inlineStr"/>
-      <c r="M101" t="inlineStr"/>
-      <c r="N101" t="inlineStr"/>
-      <c r="O101" t="inlineStr"/>
-      <c r="P101" t="inlineStr"/>
-      <c r="Q101" t="inlineStr"/>
-      <c r="R101" t="inlineStr"/>
-      <c r="S101" t="inlineStr"/>
+      <c r="L101" t="inlineStr">
+        <is>
+          <t>所得税费用</t>
+        </is>
+      </c>
+      <c r="M101" t="inlineStr">
+        <is>
+          <t>当前所得税费用</t>
+        </is>
+      </c>
+      <c r="N101" t="n">
+        <v>0</v>
+      </c>
+      <c r="O101" t="inlineStr">
+        <is>
+          <t>2021年</t>
+        </is>
+      </c>
+      <c r="P101" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q101" t="inlineStr">
+        <is>
+          <t>当前所得税费用</t>
+        </is>
+      </c>
+      <c r="R101" t="n">
+        <v>0</v>
+      </c>
+      <c r="S101" t="inlineStr">
+        <is>
+          <t>2022年</t>
+        </is>
+      </c>
     </row>
     <row r="102">
       <c r="A102" s="1" t="n">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B102" t="inlineStr">
         <is>
@@ -3259,7 +4135,7 @@
     </row>
     <row r="103">
       <c r="A103" s="1" t="n">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B103" t="inlineStr">
         <is>
@@ -3286,7 +4162,7 @@
     </row>
     <row r="104">
       <c r="A104" s="1" t="n">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B104" t="inlineStr">
         <is>
@@ -3313,7 +4189,7 @@
     </row>
     <row r="105">
       <c r="A105" s="1" t="n">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B105" t="inlineStr">
         <is>
@@ -3340,7 +4216,7 @@
     </row>
     <row r="106">
       <c r="A106" s="1" t="n">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B106" t="inlineStr">
         <is>
@@ -3367,7 +4243,7 @@
     </row>
     <row r="107">
       <c r="A107" s="1" t="n">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B107" t="inlineStr">
         <is>
@@ -3394,7 +4270,7 @@
     </row>
     <row r="108">
       <c r="A108" s="1" t="n">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B108" t="inlineStr">
         <is>
@@ -3421,7 +4297,7 @@
     </row>
     <row r="109">
       <c r="A109" s="1" t="n">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B109" t="inlineStr">
         <is>
@@ -3448,7 +4324,7 @@
     </row>
     <row r="110">
       <c r="A110" s="1" t="n">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B110" t="inlineStr">
         <is>
@@ -3475,7 +4351,7 @@
     </row>
     <row r="111">
       <c r="A111" s="1" t="n">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B111" t="inlineStr">
         <is>
@@ -3502,7 +4378,7 @@
     </row>
     <row r="112">
       <c r="A112" s="1" t="n">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B112" t="inlineStr">
         <is>
@@ -3529,7 +4405,7 @@
     </row>
     <row r="113">
       <c r="A113" s="1" t="n">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B113" t="inlineStr">
         <is>
@@ -3556,7 +4432,7 @@
     </row>
     <row r="114">
       <c r="A114" s="1" t="n">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B114" t="inlineStr">
         <is>
@@ -3583,7 +4459,7 @@
     </row>
     <row r="115">
       <c r="A115" s="1" t="n">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B115" t="inlineStr">
         <is>
@@ -3610,7 +4486,7 @@
     </row>
     <row r="116">
       <c r="A116" s="1" t="n">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B116" t="inlineStr">
         <is>
@@ -3637,7 +4513,7 @@
     </row>
     <row r="117">
       <c r="A117" s="1" t="n">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B117" t="inlineStr">
         <is>
@@ -3664,7 +4540,7 @@
     </row>
     <row r="118">
       <c r="A118" s="1" t="n">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B118" t="inlineStr">
         <is>
@@ -3691,7 +4567,7 @@
     </row>
     <row r="119">
       <c r="A119" s="1" t="n">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B119" t="inlineStr">
         <is>
@@ -3718,7 +4594,7 @@
     </row>
     <row r="120">
       <c r="A120" s="1" t="n">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B120" t="inlineStr">
         <is>
@@ -3745,7 +4621,7 @@
     </row>
     <row r="121">
       <c r="A121" s="1" t="n">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B121" t="inlineStr">
         <is>
@@ -3772,7 +4648,7 @@
     </row>
     <row r="122">
       <c r="A122" s="1" t="n">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B122" t="inlineStr">
         <is>
@@ -3799,7 +4675,7 @@
     </row>
     <row r="123">
       <c r="A123" s="1" t="n">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B123" t="inlineStr">
         <is>
@@ -3826,7 +4702,7 @@
     </row>
     <row r="124">
       <c r="A124" s="1" t="n">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B124" t="inlineStr">
         <is>
@@ -3853,7 +4729,7 @@
     </row>
     <row r="125">
       <c r="A125" s="1" t="n">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B125" t="inlineStr">
         <is>
@@ -3880,7 +4756,7 @@
     </row>
     <row r="126">
       <c r="A126" s="1" t="n">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B126" t="inlineStr">
         <is>
@@ -3907,7 +4783,7 @@
     </row>
     <row r="127">
       <c r="A127" s="1" t="n">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B127" t="inlineStr">
         <is>
@@ -3934,7 +4810,7 @@
     </row>
     <row r="128">
       <c r="A128" s="1" t="n">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B128" t="inlineStr">
         <is>
@@ -3961,7 +4837,7 @@
     </row>
     <row r="129">
       <c r="A129" s="1" t="n">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B129" t="inlineStr">
         <is>
@@ -3988,7 +4864,7 @@
     </row>
     <row r="130">
       <c r="A130" s="1" t="n">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B130" t="inlineStr">
         <is>
@@ -4015,7 +4891,7 @@
     </row>
     <row r="131">
       <c r="A131" s="1" t="n">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B131" t="inlineStr">
         <is>
@@ -4042,7 +4918,7 @@
     </row>
     <row r="132">
       <c r="A132" s="1" t="n">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B132" t="inlineStr">
         <is>
@@ -4069,7 +4945,7 @@
     </row>
     <row r="133">
       <c r="A133" s="1" t="n">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B133" t="inlineStr">
         <is>
@@ -4096,7 +4972,7 @@
     </row>
     <row r="134">
       <c r="A134" s="1" t="n">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B134" t="inlineStr">
         <is>
@@ -4123,7 +4999,7 @@
     </row>
     <row r="135">
       <c r="A135" s="1" t="n">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B135" t="inlineStr">
         <is>
@@ -4150,7 +5026,7 @@
     </row>
     <row r="136">
       <c r="A136" s="1" t="n">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B136" t="inlineStr">
         <is>
@@ -4177,7 +5053,7 @@
     </row>
     <row r="137">
       <c r="A137" s="1" t="n">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B137" t="inlineStr">
         <is>
@@ -4204,7 +5080,7 @@
     </row>
     <row r="138">
       <c r="A138" s="1" t="n">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B138" t="inlineStr">
         <is>

</xml_diff>